<commit_message>
Added random_select to quizes and enhance randomization
</commit_message>
<xml_diff>
--- a/examples/attendance_template.xlsx
+++ b/examples/attendance_template.xlsx
@@ -20,21 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t xml:space="preserve">*إسمك بالعربية كما في بطاقة الرقم القومي</t>
-  </si>
-  <si>
-    <t xml:space="preserve">answers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select</t>
+    <t xml:space="preserve">*Your Name</t>
   </si>
   <si>
     <t xml:space="preserve">#TEXT#</t>
   </si>
   <si>
-    <t xml:space="preserve">left empty in answers</t>
+    <t xml:space="preserve">Choose types whether #TEXT# or #NUMBER#</t>
   </si>
 </sst>
 </file>
@@ -153,40 +147,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1007" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>